<commit_message>
I don't know which file got missed. this time ticked every file
</commit_message>
<xml_diff>
--- a/com.blackout.solarpanelcalculator/docs/SolarPanelsInvertersBatteriesControllers.xlsx
+++ b/com.blackout.solarpanelcalculator/docs/SolarPanelsInvertersBatteriesControllers.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="144" windowWidth="22980" windowHeight="9804"/>
+    <workbookView xWindow="0" yWindow="3312" windowWidth="12636" windowHeight="5292"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -132,7 +133,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -209,11 +210,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -519,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -886,15 +887,15 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:7" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>